<commit_message>
add ip checking from firebase
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D261B6-70BD-4FDC-A08C-B706180F0834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99766B0B-2D9F-40E0-9F41-3B6C9073B60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>Employee Name</t>
   </si>
   <si>
-    <t>Office</t>
-  </si>
-  <si>
     <t>Call reason</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>Objectif</t>
+  </si>
+  <si>
+    <t>Qualification ID</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <dimension ref="A1:AM59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,126 +854,126 @@
   <sheetData>
     <row r="1" spans="1:39" ht="78" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>

</xml_diff>